<commit_message>
Support I18N for report
</commit_message>
<xml_diff>
--- a/nts.uk/shr/nts.uk.shr.com/src/main/resources/report/SampleReport.xlsx
+++ b/nts.uk/shr/nts.uk.shr.com/src/main/resources/report/SampleReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\biz\Work\Dev\Universal\Code\UniversalK\Green\nts.uk\shr\nts.uk.shr.com\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manhnd\Documents\UniversalK\nts.uk\shr\nts.uk.shr.com\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,13 +30,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>名称</t>
-    <rPh sb="0" eb="2">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>&amp;=item.code</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -45,7 +38,11 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>こーど</t>
+    <t>&amp;=I18N.Code(bean)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&amp;=I18N.Name(bean)</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -53,7 +50,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,104 +448,104 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="39.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="28.35" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="20.85" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:2" ht="20.85" customHeight="1">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="20.85" customHeight="1">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="20.85" customHeight="1">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="20.85" customHeight="1">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="20.85" customHeight="1">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="20.85" customHeight="1">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="20.85" customHeight="1">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="20.85" customHeight="1">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="20.85" customHeight="1">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" ht="20.85" customHeight="1">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" ht="20.85" customHeight="1">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" ht="20.85" customHeight="1">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" ht="20.85" customHeight="1">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:2" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" ht="20.85" customHeight="1">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" ht="20.85" customHeight="1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" ht="20.85" customHeight="1">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" ht="20.85" customHeight="1">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1" ht="20.85" customHeight="1">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1" ht="20.85" customHeight="1">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:1" ht="20.85" customHeight="1">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" ht="20.85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1" ht="20.85" customHeight="1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="33" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="1:1" ht="20.25" customHeight="1"/>
+    <row r="25" spans="1:1" ht="20.25" customHeight="1"/>
+    <row r="26" spans="1:1" ht="20.25" customHeight="1"/>
+    <row r="27" spans="1:1" ht="20.25" customHeight="1"/>
+    <row r="28" spans="1:1" ht="20.25" customHeight="1"/>
+    <row r="29" spans="1:1" ht="20.25" customHeight="1"/>
+    <row r="30" spans="1:1" ht="20.25" customHeight="1"/>
+    <row r="31" spans="1:1" ht="20.25" customHeight="1"/>
+    <row r="32" spans="1:1" ht="20.25" customHeight="1"/>
+    <row r="33" ht="20.25" customHeight="1"/>
+    <row r="34" ht="20.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.47244094488188981" right="0.47244094488188981" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>